<commit_message>
added refrence number and split payment table
</commit_message>
<xml_diff>
--- a/excel/repayment_schedule_RTN060.xlsx
+++ b/excel/repayment_schedule_RTN060.xlsx
@@ -406,10 +406,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>45052</v>
+        <v>44959</v>
       </c>
       <c r="C2">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -417,10 +417,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>45083</v>
+        <v>44987</v>
       </c>
       <c r="C3">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>45113</v>
+        <v>45018</v>
       </c>
       <c r="C4">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -439,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>45144</v>
+        <v>45048</v>
       </c>
       <c r="C5">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -450,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>45175</v>
+        <v>45079</v>
       </c>
       <c r="C6">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -461,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>45205</v>
+        <v>45109</v>
       </c>
       <c r="C7">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -472,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>45236</v>
+        <v>45140</v>
       </c>
       <c r="C8">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -483,10 +483,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>45266</v>
+        <v>45171</v>
       </c>
       <c r="C9">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -494,10 +494,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>45297</v>
+        <v>45201</v>
       </c>
       <c r="C10">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -505,10 +505,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>45328</v>
+        <v>45232</v>
       </c>
       <c r="C11">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -516,10 +516,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>45357</v>
+        <v>45262</v>
       </c>
       <c r="C12">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -527,10 +527,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>45388</v>
+        <v>45293</v>
       </c>
       <c r="C13">
-        <v>91666.66666666667</v>
+        <v>45833.33333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>